<commit_message>
Major work done on the Data Narrative, Started PPT
</commit_message>
<xml_diff>
--- a/student_info.xlsx
+++ b/student_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyled\Desktop\master_defense\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyled\Documents\GitHub\masters_defense\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73ECA836-0885-4DA1-AA21-595C3D83838A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F222E505-1B40-41E5-A6DD-A518E9416914}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="4275" windowWidth="13830" windowHeight="7170" xr2:uid="{D863DC80-1B58-44F9-9F90-EEC4AF117B2B}"/>
+    <workbookView xWindow="1365" yWindow="1335" windowWidth="26595" windowHeight="13965" xr2:uid="{D863DC80-1B58-44F9-9F90-EEC4AF117B2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="41">
   <si>
     <t>name</t>
   </si>
@@ -144,13 +144,28 @@
   </si>
   <si>
     <t>previous_course_grade</t>
+  </si>
+  <si>
+    <t>race</t>
+  </si>
+  <si>
+    <t>latinx</t>
+  </si>
+  <si>
+    <t>african american</t>
+  </si>
+  <si>
+    <t>african</t>
+  </si>
+  <si>
+    <t>brazilian</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +175,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -184,15 +206,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -504,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A294BDE2-7C19-48D5-A479-50D11FEDD38E}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="H1" sqref="G1:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +543,7 @@
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -531,8 +556,11 @@
       <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -545,8 +573,12 @@
       <c r="D2">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -559,8 +591,12 @@
       <c r="D3">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -573,8 +609,12 @@
       <c r="D4">
         <v>76</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -587,8 +627,11 @@
       <c r="D5">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -601,8 +644,11 @@
       <c r="D6">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -615,8 +661,11 @@
       <c r="D7">
         <v>83</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -629,8 +678,11 @@
       <c r="D8">
         <v>89</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -643,8 +695,11 @@
       <c r="D9">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -657,8 +712,11 @@
       <c r="D10">
         <v>75</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -671,8 +729,11 @@
       <c r="D11">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -685,8 +746,11 @@
       <c r="D12">
         <v>88</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -699,8 +763,11 @@
       <c r="D13">
         <v>94</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -713,8 +780,11 @@
       <c r="D14">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -727,8 +797,11 @@
       <c r="D15">
         <v>72</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -741,8 +814,11 @@
       <c r="D16">
         <v>81</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -755,8 +831,11 @@
       <c r="D17">
         <v>83</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -769,8 +848,11 @@
       <c r="D18">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -783,8 +865,11 @@
       <c r="D19">
         <v>91</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -797,8 +882,11 @@
       <c r="D20">
         <v>90</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -811,8 +899,11 @@
       <c r="D21">
         <v>89</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -825,8 +916,11 @@
       <c r="D22">
         <v>75</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -839,8 +933,11 @@
       <c r="D23">
         <v>80</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -853,8 +950,11 @@
       <c r="D24">
         <v>88</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>19</v>
       </c>
@@ -867,8 +967,11 @@
       <c r="D25">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -881,8 +984,11 @@
       <c r="D26">
         <v>80</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -895,8 +1001,11 @@
       <c r="D27">
         <v>79</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>7</v>
       </c>
@@ -909,8 +1018,11 @@
       <c r="D28">
         <v>86</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -923,8 +1035,11 @@
       <c r="D29">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -937,8 +1052,11 @@
       <c r="D30">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -950,6 +1068,9 @@
       </c>
       <c r="D31">
         <v>68</v>
+      </c>
+      <c r="E31" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>